<commit_message>
update: keep track of the old priority in old_index
</commit_message>
<xml_diff>
--- a/master_spreadsheet_summer_25_26.xlsx
+++ b/master_spreadsheet_summer_25_26.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\Test\function\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B89924-DAA4-480B-909B-79954CBBD5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A6DF0-B7C5-4268-838E-2F38866448D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2916" yWindow="2652" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Source ID</t>
   </si>
@@ -149,13 +149,16 @@
   </si>
   <si>
     <t>E015</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +187,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -216,11 +226,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
@@ -235,6 +269,26 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -519,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -774,239 +828,293 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB045595-88CF-4B1B-827F-6138CF5A9DC8}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="55.8" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="43.8" thickBot="1">
+      <c r="A1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" ht="15" thickBot="1">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="7">
         <v>5000</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="8">
         <v>45703</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="7">
         <v>8000</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="8">
         <v>45708</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="7">
         <v>3000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="8">
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="7">
         <v>12000</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="8">
         <v>45762</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="7">
         <v>15000</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="8">
         <v>45797</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" ht="15" thickBot="1">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="7">
         <v>4000</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="8">
         <v>45818</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="7">
         <v>8000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="8">
         <v>45853</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="7">
         <v>10000</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="8">
         <v>45858</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="7">
         <v>6000</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="8">
         <v>45879</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:5" ht="15" thickBot="1">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
+      <c r="D11" s="7">
         <v>15000</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="8">
         <v>45915</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D12" s="7">
         <v>12000</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="8">
         <v>45950</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:5" ht="15" thickBot="1">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D13" s="7">
         <v>5000</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="8">
         <v>45971</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="7">
         <v>10000</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="8">
         <v>46006</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" thickBot="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:5" ht="29.4" thickBot="1">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5">
+      <c r="D15" s="7">
         <v>20000</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="8">
         <v>46011</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5">
+      <c r="D16" s="12">
         <v>15000</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="13">
         <v>46016</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: download current data as Excel file
</commit_message>
<xml_diff>
--- a/master_spreadsheet_summer_25_26.xlsx
+++ b/master_spreadsheet_summer_25_26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A6DF0-B7C5-4268-838E-2F38866448D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5AF94-8504-4E2B-8299-A6698D557DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Source ID</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -167,13 +170,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -183,16 +179,24 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -211,86 +215,37 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -583,29 +538,32 @@
     <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="43.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4">
@@ -617,13 +575,13 @@
       <c r="E2" s="5">
         <v>15000</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="28.2" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="4">
@@ -635,13 +593,13 @@
       <c r="E3" s="5">
         <v>12000</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4">
@@ -653,13 +611,13 @@
       <c r="E4" s="5">
         <v>8000</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.2" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.8">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4">
@@ -671,13 +629,13 @@
       <c r="E5" s="5">
         <v>20000</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="42" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.8">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4">
@@ -689,13 +647,13 @@
       <c r="E6" s="5">
         <v>10000</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="4">
@@ -707,13 +665,13 @@
       <c r="E7" s="5">
         <v>18000</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.2" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.8">
+      <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="4">
@@ -725,13 +683,13 @@
       <c r="E8" s="5">
         <v>25000</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="4">
@@ -743,13 +701,13 @@
       <c r="E9" s="5">
         <v>5000</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="42" thickBot="1">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="43.2">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="4">
@@ -761,13 +719,13 @@
       <c r="E10" s="5">
         <v>14000</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="55.8" thickBot="1">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="43.2">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="4">
@@ -779,47 +737,47 @@
       <c r="E11" s="5">
         <v>10000</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -828,288 +786,293 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB045595-88CF-4B1B-827F-6138CF5A9DC8}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="6"/>
+    <col min="4" max="4" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.8" thickBot="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" ht="43.2">
+      <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1">
-      <c r="A2" s="9">
+      <c r="F1" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>5000</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="4">
         <v>45703</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A3" s="9">
+    <row r="3" spans="1:6" ht="28.8">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>8000</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>45708</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
-      <c r="A4" s="9">
+    <row r="4" spans="1:6">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>3000</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
-      <c r="A5" s="9">
+    <row r="5" spans="1:6">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>12000</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>45762</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A6" s="9">
+    <row r="6" spans="1:6" ht="28.8">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>15000</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <v>45797</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
-      <c r="A7" s="9">
+    <row r="7" spans="1:6">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>4000</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <v>45818</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
-      <c r="A8" s="9">
+    <row r="8" spans="1:6">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>8000</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <v>45853</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A9" s="9">
+    <row r="9" spans="1:6" ht="28.8">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>10000</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>45858</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1">
-      <c r="A10" s="9">
+    <row r="10" spans="1:6">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>6000</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>45879</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
-      <c r="A11" s="9">
+    <row r="11" spans="1:6">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>15000</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="4">
         <v>45915</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A12" s="9">
+    <row r="12" spans="1:6" ht="28.8">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>12000</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="4">
         <v>45950</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
-      <c r="A13" s="9">
+    <row r="13" spans="1:6">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>5000</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>45971</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1">
-      <c r="A14" s="9">
+    <row r="14" spans="1:6">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>10000</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>46006</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29.4" thickBot="1">
-      <c r="A15" s="9">
+    <row r="15" spans="1:6" ht="28.8">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>20000</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>46011</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="10">
+    <row r="16" spans="1:6">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="5">
         <v>15000</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="4">
         <v>46016</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: adding expense name to the masterspreadsheet
</commit_message>
<xml_diff>
--- a/master_spreadsheet_summer_25_26.xlsx
+++ b/master_spreadsheet_summer_25_26.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110D7186-7B96-4100-91D7-04400D60CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5D6B51-413F-4086-9512-56F68BC82B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>Source ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Item ID</t>
-  </si>
-  <si>
     <t>Expense Category</t>
   </si>
   <si>
@@ -55,102 +52,27 @@
     <t>Latest Payment Date</t>
   </si>
   <si>
-    <t>FS001</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
-    <t>E001</t>
-  </si>
-  <si>
-    <t>FS002</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
-    <t>E002</t>
-  </si>
-  <si>
-    <t>FS003</t>
-  </si>
-  <si>
     <t>Travel</t>
   </si>
   <si>
-    <t>E003</t>
-  </si>
-  <si>
-    <t>FS004</t>
-  </si>
-  <si>
     <t>Salary, Travel</t>
   </si>
   <si>
-    <t>E004</t>
-  </si>
-  <si>
-    <t>FS005</t>
-  </si>
-  <si>
     <t>Equipment, Travel</t>
   </si>
   <si>
-    <t>E005</t>
-  </si>
-  <si>
-    <t>FS006</t>
-  </si>
-  <si>
-    <t>E006</t>
-  </si>
-  <si>
-    <t>FS007</t>
-  </si>
-  <si>
-    <t>E007</t>
-  </si>
-  <si>
-    <t>FS008</t>
-  </si>
-  <si>
-    <t>E008</t>
-  </si>
-  <si>
-    <t>FS009</t>
-  </si>
-  <si>
     <t>Salary, Equipment</t>
   </si>
   <si>
-    <t>E009</t>
-  </si>
-  <si>
-    <t>FS010</t>
-  </si>
-  <si>
     <t>Salary, Equipment, Travel</t>
   </si>
   <si>
-    <t>E010</t>
-  </si>
-  <si>
-    <t>E011</t>
-  </si>
-  <si>
-    <t>E012</t>
-  </si>
-  <si>
-    <t>E013</t>
-  </si>
-  <si>
-    <t>E014</t>
-  </si>
-  <si>
-    <t>E015</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -167,13 +89,94 @@
   </si>
   <si>
     <t>Funding Source</t>
+  </si>
+  <si>
+    <t>Expense Name</t>
+  </si>
+  <si>
+    <t>Expense ID</t>
+  </si>
+  <si>
+    <t>E-01</t>
+  </si>
+  <si>
+    <t>E-02</t>
+  </si>
+  <si>
+    <t>E-03</t>
+  </si>
+  <si>
+    <t>E-04</t>
+  </si>
+  <si>
+    <t>E-05</t>
+  </si>
+  <si>
+    <t>E-06</t>
+  </si>
+  <si>
+    <t>E-07</t>
+  </si>
+  <si>
+    <t>E-08</t>
+  </si>
+  <si>
+    <t>E-09</t>
+  </si>
+  <si>
+    <t>E-10</t>
+  </si>
+  <si>
+    <t>E-11</t>
+  </si>
+  <si>
+    <t>E-12</t>
+  </si>
+  <si>
+    <t>E-13</t>
+  </si>
+  <si>
+    <t>E-14</t>
+  </si>
+  <si>
+    <t>E-15</t>
+  </si>
+  <si>
+    <t>FS-01</t>
+  </si>
+  <si>
+    <t>FS-02</t>
+  </si>
+  <si>
+    <t>FS-03</t>
+  </si>
+  <si>
+    <t>FS-04</t>
+  </si>
+  <si>
+    <t>FS-05</t>
+  </si>
+  <si>
+    <t>FS-06</t>
+  </si>
+  <si>
+    <t>FS-07</t>
+  </si>
+  <si>
+    <t>FS-08</t>
+  </si>
+  <si>
+    <t>FS-09</t>
+  </si>
+  <si>
+    <t>FS-10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +212,12 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -535,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -552,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>1</v>
@@ -567,18 +576,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="43.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4">
         <v>45658</v>
@@ -591,15 +600,15 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="43.2">
+    <row r="3" spans="1:7" ht="28.8">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4">
         <v>45689</v>
@@ -612,15 +621,15 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="43.2">
+    <row r="4" spans="1:7" ht="28.8">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4">
         <v>45717</v>
@@ -633,15 +642,15 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="43.2">
+    <row r="5" spans="1:7" ht="28.8">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4">
         <v>45658</v>
@@ -654,15 +663,15 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="43.2">
+    <row r="6" spans="1:7" ht="28.8">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4">
         <v>45748</v>
@@ -675,15 +684,15 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="43.2">
+    <row r="7" spans="1:7" ht="28.8">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4">
         <v>45809</v>
@@ -696,15 +705,15 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="43.2">
+    <row r="8" spans="1:7" ht="28.8">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4">
         <v>45658</v>
@@ -717,15 +726,15 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="43.2">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" s="4">
         <v>45778</v>
@@ -738,15 +747,15 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="43.2">
+    <row r="10" spans="1:7" ht="28.8">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4">
         <v>45839</v>
@@ -761,13 +770,13 @@
     </row>
     <row r="11" spans="1:7" ht="43.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4">
         <v>45658</v>
@@ -826,303 +835,323 @@
       <c r="G16" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB045595-88CF-4B1B-827F-6138CF5A9DC8}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="6"/>
-    <col min="4" max="4" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="6"/>
+    <col min="2" max="4" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="9" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.2">
+    <row r="1" spans="1:7" ht="43.2">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5">
         <v>5000</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>45703</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8">
+    <row r="3" spans="1:7" ht="28.8">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5">
         <v>8000</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>45708</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5">
         <v>3000</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>45726</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
         <v>12000</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>45762</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8">
+    <row r="6" spans="1:7" ht="28.8">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5">
         <v>15000</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>45797</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5">
         <v>4000</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>45818</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5">
         <v>8000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>45853</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="5">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5">
         <v>10000</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>45858</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
         <v>6000</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>45879</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5">
         <v>15000</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>45915</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8">
+    <row r="12" spans="1:7" ht="28.8">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="5">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5">
         <v>12000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>45950</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5">
         <v>5000</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>45971</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
         <v>10000</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>46006</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8">
+    <row r="15" spans="1:7" ht="28.8">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="5">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5">
         <v>20000</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>46011</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="5">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5">
         <v>15000</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>46016</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>